<commit_message>
updating final assignment and code
</commit_message>
<xml_diff>
--- a/project_raw_data/ram.xlsx
+++ b/project_raw_data/ram.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t xml:space="preserve">Cell#</t>
   </si>
@@ -76,12 +76,6 @@
   </si>
   <si>
     <t xml:space="preserve">fk011   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">.</t>
   </si>
   <si>
     <t xml:space="preserve">fk018   </t>
@@ -546,14 +540,11 @@
   </sheetPr>
   <dimension ref="A1:Q124"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T27" activeCellId="0" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.54081632653061"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -615,17 +606,17 @@
       <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>18</v>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>-38.36</v>
@@ -654,16 +645,16 @@
       <c r="O2" s="0" t="n">
         <v>-26.95</v>
       </c>
-      <c r="P2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>19</v>
+      <c r="P2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -671,14 +662,14 @@
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>18</v>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>18</v>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>-50.83</v>
@@ -716,22 +707,22 @@
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>18</v>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>-36.52</v>
@@ -769,22 +760,22 @@
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>18</v>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>-48.34</v>
@@ -822,22 +813,22 @@
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>18</v>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>-63.99</v>
@@ -875,22 +866,22 @@
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>18</v>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>-42.95</v>
@@ -928,7 +919,7 @@
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
@@ -939,11 +930,11 @@
       <c r="D8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>18</v>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>-50.88</v>
@@ -981,7 +972,7 @@
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -992,11 +983,11 @@
       <c r="D9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>18</v>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>-45.36</v>
@@ -1034,7 +1025,7 @@
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -1048,8 +1039,8 @@
       <c r="E10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>18</v>
+      <c r="F10" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>-51.61</v>
@@ -1087,28 +1078,28 @@
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>18</v>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="0" t="s">
-        <v>18</v>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>-37.55</v>
       </c>
-      <c r="H11" s="0" t="s">
-        <v>19</v>
+      <c r="H11" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>61.13</v>
@@ -1140,22 +1131,22 @@
     </row>
     <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>18</v>
+      <c r="C12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>18</v>
+      <c r="F12" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>-44.92</v>
@@ -1193,16 +1184,16 @@
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>18</v>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>3</v>
@@ -1237,31 +1228,31 @@
       <c r="O13" s="0" t="n">
         <v>-30.03</v>
       </c>
-      <c r="P13" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="0" t="s">
-        <v>19</v>
+      <c r="P13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>18</v>
+      <c r="C14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="0" t="s">
-        <v>18</v>
+      <c r="F14" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>-36.14</v>
@@ -1269,58 +1260,58 @@
       <c r="H14" s="0" t="n">
         <v>64.74</v>
       </c>
-      <c r="I14" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>19</v>
+      <c r="I14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="M14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N14" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="P14" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="0" t="s">
-        <v>19</v>
+      <c r="N14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>18</v>
+      <c r="C15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>18</v>
+      <c r="F15" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>-44.38</v>
       </c>
-      <c r="H15" s="0" t="s">
-        <v>19</v>
+      <c r="H15" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>33.11</v>
@@ -1343,16 +1334,16 @@
       <c r="O15" s="0" t="n">
         <v>-34.91</v>
       </c>
-      <c r="P15" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q15" s="0" t="s">
-        <v>19</v>
+      <c r="P15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
@@ -1384,8 +1375,8 @@
       <c r="K16" s="0" t="n">
         <v>39.16</v>
       </c>
-      <c r="L16" s="0" t="s">
-        <v>19</v>
+      <c r="L16" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="M16" s="0" t="n">
         <v>5</v>
@@ -1405,22 +1396,22 @@
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>18</v>
+      <c r="C17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>-42.5</v>
@@ -1458,22 +1449,22 @@
     </row>
     <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>18</v>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>-58.61</v>
@@ -1511,22 +1502,22 @@
     </row>
     <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>18</v>
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>-50.75</v>
@@ -1564,22 +1555,22 @@
     </row>
     <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>18</v>
+      <c r="C20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>-42.24</v>
@@ -1617,7 +1608,7 @@
     </row>
     <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>2</v>
@@ -1628,11 +1619,11 @@
       <c r="D21" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>18</v>
+      <c r="E21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>-39.83</v>
@@ -1670,28 +1661,28 @@
     </row>
     <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>18</v>
+      <c r="C22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F22" s="0" t="s">
-        <v>18</v>
+      <c r="F22" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>-46.14</v>
       </c>
-      <c r="H22" s="0" t="s">
-        <v>19</v>
+      <c r="H22" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>60.26</v>
@@ -1723,22 +1714,22 @@
     </row>
     <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>18</v>
+      <c r="C23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>-45.81</v>
@@ -1776,7 +1767,7 @@
     </row>
     <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
@@ -1796,8 +1787,8 @@
       <c r="G24" s="0" t="n">
         <v>-67.98</v>
       </c>
-      <c r="H24" s="0" t="s">
-        <v>19</v>
+      <c r="H24" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>54.61</v>
@@ -1829,22 +1820,22 @@
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>18</v>
+      <c r="C25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>-70.48</v>
@@ -1882,22 +1873,22 @@
     </row>
     <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>18</v>
+      <c r="C26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>-34.09</v>
@@ -1935,22 +1926,22 @@
     </row>
     <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>18</v>
+      <c r="C27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>-56.25</v>
@@ -1988,22 +1979,22 @@
     </row>
     <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>18</v>
+      <c r="C28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>-64.24</v>
@@ -2041,7 +2032,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>3</v>
@@ -2049,14 +2040,14 @@
       <c r="C29" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>18</v>
+      <c r="D29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>-87.72</v>
@@ -2094,7 +2085,7 @@
     </row>
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>3</v>
@@ -2105,11 +2096,11 @@
       <c r="D30" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E30" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>18</v>
+      <c r="E30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>-66.3</v>
@@ -2147,22 +2138,22 @@
     </row>
     <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>18</v>
+      <c r="C31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>-69.84</v>
@@ -2200,22 +2191,22 @@
     </row>
     <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>18</v>
+      <c r="C32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>-68.11</v>
@@ -2253,7 +2244,7 @@
     </row>
     <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>3</v>
@@ -2264,11 +2255,11 @@
       <c r="D33" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E33" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>18</v>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>-82.78</v>
@@ -2306,7 +2297,7 @@
     </row>
     <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>3</v>
@@ -2317,11 +2308,11 @@
       <c r="D34" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E34" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>18</v>
+      <c r="E34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>-59.46</v>
@@ -2359,22 +2350,22 @@
     </row>
     <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>18</v>
+      <c r="C35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G35" s="0" t="n">
         <v>-76.06</v>
@@ -2412,22 +2403,22 @@
     </row>
     <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>18</v>
+      <c r="C36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>-70.27</v>
@@ -2465,22 +2456,22 @@
     </row>
     <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C37" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>18</v>
+      <c r="C37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G37" s="0" t="n">
         <v>-59.44</v>
@@ -2518,22 +2509,22 @@
     </row>
     <row r="38" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C38" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>18</v>
+      <c r="C38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G38" s="0" t="n">
         <v>-66.96</v>
@@ -2571,7 +2562,7 @@
     </row>
     <row r="39" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>3</v>
@@ -2582,11 +2573,11 @@
       <c r="D39" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E39" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>18</v>
+      <c r="E39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G39" s="0" t="n">
         <v>-56.45</v>
@@ -2624,22 +2615,22 @@
     </row>
     <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C40" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>18</v>
+      <c r="C40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G40" s="0" t="n">
         <v>-58.2</v>
@@ -2677,22 +2668,22 @@
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C41" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>18</v>
+      <c r="C41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G41" s="0" t="n">
         <v>-69.34</v>
@@ -2730,28 +2721,28 @@
     </row>
     <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>19</v>
+      <c r="C42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>55.56</v>
@@ -2783,16 +2774,16 @@
     </row>
     <row r="43" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C43" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>18</v>
+      <c r="C43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>1</v>
@@ -2836,22 +2827,22 @@
     </row>
     <row r="44" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C44" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>18</v>
+      <c r="C44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F44" s="0" t="s">
-        <v>18</v>
+      <c r="F44" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G44" s="0" t="n">
         <v>-53.96</v>
@@ -2889,28 +2880,28 @@
     </row>
     <row r="45" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C45" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>18</v>
+      <c r="C45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F45" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>19</v>
+      <c r="F45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>50.65</v>
@@ -2933,25 +2924,25 @@
       <c r="O45" s="0" t="n">
         <v>-55.13</v>
       </c>
-      <c r="P45" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q45" s="0" t="s">
-        <v>19</v>
+      <c r="P45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>18</v>
+      <c r="C46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>1</v>
@@ -2959,11 +2950,11 @@
       <c r="F46" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G46" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H46" s="0" t="s">
-        <v>19</v>
+      <c r="G46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>57.51</v>
@@ -2995,16 +2986,16 @@
     </row>
     <row r="47" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C47" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>18</v>
+      <c r="C47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>2</v>
@@ -3018,46 +3009,46 @@
       <c r="H47" s="0" t="n">
         <v>42.08</v>
       </c>
-      <c r="I47" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J47" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K47" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="L47" s="0" t="s">
-        <v>19</v>
+      <c r="I47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="M47" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N47" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="O47" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="P47" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q47" s="0" t="s">
-        <v>19</v>
+      <c r="N47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>18</v>
+      <c r="C48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>3</v>
@@ -3101,7 +3092,7 @@
     </row>
     <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>3</v>
@@ -3154,22 +3145,22 @@
     </row>
     <row r="50" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C50" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F50" s="0" t="s">
-        <v>18</v>
+      <c r="C50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G50" s="0" t="n">
         <v>-59.08</v>
@@ -3207,22 +3198,22 @@
     </row>
     <row r="51" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C51" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>18</v>
+      <c r="C51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G51" s="0" t="n">
         <v>-48.95</v>
@@ -3260,22 +3251,22 @@
     </row>
     <row r="52" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C52" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>18</v>
+      <c r="C52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G52" s="0" t="n">
         <v>-51.94</v>
@@ -3313,16 +3304,16 @@
     </row>
     <row r="53" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C53" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>18</v>
+      <c r="C53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>2</v>
@@ -3366,16 +3357,16 @@
     </row>
     <row r="54" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C54" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>18</v>
+      <c r="C54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>2</v>
@@ -3419,22 +3410,22 @@
     </row>
     <row r="55" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C55" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>18</v>
+      <c r="C55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F55" s="0" t="s">
-        <v>18</v>
+      <c r="F55" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G55" s="0" t="n">
         <v>-56.55</v>
@@ -3472,16 +3463,16 @@
     </row>
     <row r="56" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C56" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>18</v>
+      <c r="C56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>2</v>
@@ -3525,16 +3516,16 @@
     </row>
     <row r="57" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C57" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>18</v>
+      <c r="C57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>3</v>
@@ -3578,16 +3569,16 @@
     </row>
     <row r="58" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C58" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>18</v>
+      <c r="C58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>2</v>
@@ -3601,29 +3592,29 @@
       <c r="H58" s="0" t="n">
         <v>49.11</v>
       </c>
-      <c r="I58" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J58" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K58" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="L58" s="0" t="s">
-        <v>19</v>
+      <c r="I58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="M58" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N58" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="O58" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="P58" s="0" t="s">
-        <v>19</v>
+      <c r="N58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="Q58" s="0" t="n">
         <v>27</v>
@@ -3631,22 +3622,22 @@
     </row>
     <row r="59" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C59" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>18</v>
+      <c r="C59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F59" s="0" t="s">
-        <v>18</v>
+      <c r="F59" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G59" s="0" t="n">
         <v>-54.22</v>
@@ -3684,7 +3675,7 @@
     </row>
     <row r="60" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>3</v>
@@ -3695,17 +3686,17 @@
       <c r="D60" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E60" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G60" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H60" s="0" t="s">
-        <v>19</v>
+      <c r="E60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I60" s="0" t="n">
         <v>67.46</v>
@@ -3728,16 +3719,16 @@
       <c r="O60" s="0" t="n">
         <v>-49.32</v>
       </c>
-      <c r="P60" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q60" s="0" t="s">
-        <v>19</v>
+      <c r="P60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>3</v>
@@ -3751,8 +3742,8 @@
       <c r="E61" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F61" s="0" t="s">
-        <v>18</v>
+      <c r="F61" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G61" s="0" t="n">
         <v>-49.73</v>
@@ -3790,22 +3781,22 @@
     </row>
     <row r="62" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C62" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>18</v>
+      <c r="C62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F62" s="0" t="s">
-        <v>18</v>
+      <c r="F62" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G62" s="0" t="n">
         <v>-56.46</v>
@@ -3843,22 +3834,22 @@
     </row>
     <row r="63" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C63" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>18</v>
+      <c r="C63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F63" s="0" t="s">
-        <v>18</v>
+      <c r="F63" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G63" s="0" t="n">
         <v>-68.17</v>
@@ -3896,16 +3887,16 @@
     </row>
     <row r="64" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C64" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>18</v>
+      <c r="C64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>3</v>
@@ -3940,31 +3931,31 @@
       <c r="O64" s="0" t="n">
         <v>-53.08</v>
       </c>
-      <c r="P64" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q64" s="0" t="s">
-        <v>19</v>
+      <c r="P64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C65" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F65" s="0" t="s">
-        <v>18</v>
+      <c r="C65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G65" s="0" t="n">
         <v>-54.67</v>
@@ -3993,31 +3984,31 @@
       <c r="O65" s="0" t="n">
         <v>-38.79</v>
       </c>
-      <c r="P65" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q65" s="0" t="s">
-        <v>19</v>
+      <c r="P65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C66" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F66" s="0" t="s">
-        <v>18</v>
+      <c r="C66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G66" s="0" t="n">
         <v>-61.22</v>
@@ -4055,22 +4046,22 @@
     </row>
     <row r="67" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C67" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F67" s="0" t="s">
-        <v>18</v>
+      <c r="C67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G67" s="0" t="n">
         <v>-64.02</v>
@@ -4108,28 +4099,28 @@
     </row>
     <row r="68" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C68" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F68" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G68" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H68" s="0" t="s">
-        <v>19</v>
+      <c r="C68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I68" s="0" t="n">
         <v>49.02</v>
@@ -4152,31 +4143,31 @@
       <c r="O68" s="0" t="n">
         <v>-46.75</v>
       </c>
-      <c r="P68" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q68" s="0" t="s">
-        <v>19</v>
+      <c r="P68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C69" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>18</v>
+      <c r="C69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G69" s="0" t="n">
         <v>-58.89</v>
@@ -4214,22 +4205,22 @@
     </row>
     <row r="70" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C70" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F70" s="0" t="s">
-        <v>18</v>
+      <c r="C70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G70" s="0" t="n">
         <v>-59.82</v>
@@ -4267,22 +4258,22 @@
     </row>
     <row r="71" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C71" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F71" s="0" t="s">
-        <v>18</v>
+      <c r="C71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G71" s="0" t="n">
         <v>-57.05</v>
@@ -4320,7 +4311,7 @@
     </row>
     <row r="72" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>3</v>
@@ -4328,8 +4319,8 @@
       <c r="C72" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D72" s="0" t="s">
-        <v>18</v>
+      <c r="D72" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>1</v>
@@ -4373,22 +4364,22 @@
     </row>
     <row r="73" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C73" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E73" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F73" s="0" t="s">
-        <v>18</v>
+      <c r="C73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G73" s="0" t="n">
         <v>-60.45</v>
@@ -4426,28 +4417,28 @@
     </row>
     <row r="74" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C74" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F74" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G74" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H74" s="0" t="s">
-        <v>19</v>
+      <c r="C74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I74" s="0" t="n">
         <v>58.69</v>
@@ -4470,31 +4461,31 @@
       <c r="O74" s="0" t="n">
         <v>-49.07</v>
       </c>
-      <c r="P74" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q74" s="0" t="s">
-        <v>19</v>
+      <c r="P74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C75" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F75" s="0" t="s">
-        <v>18</v>
+      <c r="C75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G75" s="0" t="n">
         <v>-58.48</v>
@@ -4523,31 +4514,31 @@
       <c r="O75" s="0" t="n">
         <v>-47.59</v>
       </c>
-      <c r="P75" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q75" s="0" t="s">
-        <v>19</v>
+      <c r="P75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q75" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C76" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E76" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F76" s="0" t="s">
-        <v>18</v>
+      <c r="C76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G76" s="0" t="n">
         <v>-61.14</v>
@@ -4576,31 +4567,31 @@
       <c r="O76" s="0" t="n">
         <v>-48.68</v>
       </c>
-      <c r="P76" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q76" s="0" t="s">
-        <v>19</v>
+      <c r="P76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q76" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C77" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E77" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F77" s="0" t="s">
-        <v>18</v>
+      <c r="C77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G77" s="0" t="n">
         <v>-52.15</v>
@@ -4638,22 +4629,22 @@
     </row>
     <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C78" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F78" s="0" t="s">
-        <v>18</v>
+      <c r="C78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G78" s="0" t="n">
         <v>-60.91</v>
@@ -4691,7 +4682,7 @@
     </row>
     <row r="79" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>4</v>
@@ -4702,11 +4693,11 @@
       <c r="D79" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E79" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F79" s="0" t="s">
-        <v>18</v>
+      <c r="E79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G79" s="0" t="n">
         <v>-67.26</v>
@@ -4744,22 +4735,22 @@
     </row>
     <row r="80" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C80" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D80" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E80" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F80" s="0" t="s">
-        <v>18</v>
+      <c r="C80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G80" s="0" t="n">
         <v>-56.97</v>
@@ -4797,22 +4788,22 @@
     </row>
     <row r="81" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C81" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D81" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E81" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F81" s="0" t="s">
-        <v>18</v>
+      <c r="C81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G81" s="0" t="n">
         <v>-57.23</v>
@@ -4850,22 +4841,22 @@
     </row>
     <row r="82" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C82" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E82" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F82" s="0" t="s">
-        <v>18</v>
+      <c r="C82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G82" s="0" t="n">
         <v>-56.24</v>
@@ -4903,22 +4894,22 @@
     </row>
     <row r="83" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C83" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E83" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F83" s="0" t="s">
-        <v>18</v>
+      <c r="C83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G83" s="0" t="n">
         <v>-68.93</v>
@@ -4956,22 +4947,22 @@
     </row>
     <row r="84" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C84" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E84" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F84" s="0" t="s">
-        <v>18</v>
+      <c r="C84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G84" s="0" t="n">
         <v>-58.49</v>
@@ -5000,16 +4991,16 @@
       <c r="O84" s="0" t="n">
         <v>-46.53</v>
       </c>
-      <c r="P84" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q84" s="0" t="s">
-        <v>19</v>
+      <c r="P84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q84" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>4</v>
@@ -5020,11 +5011,11 @@
       <c r="D85" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E85" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F85" s="0" t="s">
-        <v>18</v>
+      <c r="E85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G85" s="0" t="n">
         <v>-64.03</v>
@@ -5062,7 +5053,7 @@
     </row>
     <row r="86" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>4</v>
@@ -5073,11 +5064,11 @@
       <c r="D86" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E86" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F86" s="0" t="s">
-        <v>18</v>
+      <c r="E86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G86" s="0" t="n">
         <v>-45.25</v>
@@ -5115,22 +5106,22 @@
     </row>
     <row r="87" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C87" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D87" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E87" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F87" s="0" t="s">
-        <v>18</v>
+      <c r="C87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G87" s="0" t="n">
         <v>-69.71</v>
@@ -5138,26 +5129,26 @@
       <c r="H87" s="0" t="n">
         <v>100.51</v>
       </c>
-      <c r="I87" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J87" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K87" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="L87" s="0" t="s">
-        <v>19</v>
+      <c r="I87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L87" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="M87" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="N87" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="O87" s="0" t="s">
-        <v>19</v>
+      <c r="N87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O87" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="P87" s="0" t="n">
         <v>38</v>
@@ -5168,22 +5159,22 @@
     </row>
     <row r="88" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C88" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D88" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E88" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F88" s="0" t="s">
-        <v>18</v>
+      <c r="C88" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F88" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G88" s="0" t="n">
         <v>-60.96</v>
@@ -5221,7 +5212,7 @@
     </row>
     <row r="89" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>4</v>
@@ -5232,11 +5223,11 @@
       <c r="D89" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E89" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F89" s="0" t="s">
-        <v>18</v>
+      <c r="E89" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F89" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G89" s="0" t="n">
         <v>-59.42</v>
@@ -5274,7 +5265,7 @@
     </row>
     <row r="90" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>4</v>
@@ -5285,11 +5276,11 @@
       <c r="D90" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E90" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F90" s="0" t="s">
-        <v>18</v>
+      <c r="E90" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G90" s="0" t="n">
         <v>-52.27</v>
@@ -5297,26 +5288,26 @@
       <c r="H90" s="0" t="n">
         <v>79.01</v>
       </c>
-      <c r="I90" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J90" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K90" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="L90" s="0" t="s">
-        <v>19</v>
+      <c r="I90" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K90" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L90" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="M90" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="N90" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="O90" s="0" t="s">
-        <v>19</v>
+      <c r="N90" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O90" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="P90" s="0" t="n">
         <v>40</v>
@@ -5327,7 +5318,7 @@
     </row>
     <row r="91" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>4</v>
@@ -5338,11 +5329,11 @@
       <c r="D91" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E91" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F91" s="0" t="s">
-        <v>18</v>
+      <c r="E91" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G91" s="0" t="n">
         <v>-69.68</v>
@@ -5380,22 +5371,22 @@
     </row>
     <row r="92" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C92" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D92" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E92" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F92" s="0" t="s">
-        <v>18</v>
+      <c r="C92" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G92" s="0" t="n">
         <v>-58.79</v>
@@ -5433,22 +5424,22 @@
     </row>
     <row r="93" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C93" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D93" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E93" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F93" s="0" t="s">
-        <v>18</v>
+      <c r="C93" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G93" s="0" t="n">
         <v>-70.56</v>
@@ -5486,22 +5477,22 @@
     </row>
     <row r="94" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C94" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D94" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E94" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F94" s="0" t="s">
-        <v>18</v>
+      <c r="C94" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F94" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G94" s="0" t="n">
         <v>-51.56</v>
@@ -5539,22 +5530,22 @@
     </row>
     <row r="95" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C95" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D95" s="0" t="s">
-        <v>18</v>
+      <c r="C95" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F95" s="0" t="s">
-        <v>18</v>
+      <c r="F95" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G95" s="0" t="n">
         <v>-60.3</v>
@@ -5592,22 +5583,22 @@
     </row>
     <row r="96" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C96" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D96" s="0" t="s">
-        <v>18</v>
+      <c r="C96" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F96" s="0" t="s">
-        <v>18</v>
+      <c r="F96" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G96" s="0" t="n">
         <v>-66.47</v>
@@ -5645,16 +5636,16 @@
     </row>
     <row r="97" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C97" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D97" s="0" t="s">
-        <v>18</v>
+      <c r="C97" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>2</v>
@@ -5698,7 +5689,7 @@
     </row>
     <row r="98" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>4</v>
@@ -5712,8 +5703,8 @@
       <c r="E98" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F98" s="0" t="s">
-        <v>18</v>
+      <c r="F98" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G98" s="0" t="n">
         <v>-56.35</v>
@@ -5751,28 +5742,28 @@
     </row>
     <row r="99" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C99" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D99" s="0" t="s">
-        <v>18</v>
+      <c r="C99" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E99" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F99" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G99" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H99" s="0" t="s">
-        <v>19</v>
+      <c r="F99" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H99" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I99" s="0" t="n">
         <v>26.16</v>
@@ -5795,25 +5786,25 @@
       <c r="O99" s="0" t="n">
         <v>-35.36</v>
       </c>
-      <c r="P99" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q99" s="0" t="s">
-        <v>19</v>
+      <c r="P99" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q99" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C100" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D100" s="0" t="s">
-        <v>18</v>
+      <c r="C100" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D100" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>1</v>
@@ -5848,37 +5839,37 @@
       <c r="O100" s="0" t="n">
         <v>-37.8</v>
       </c>
-      <c r="P100" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q100" s="0" t="s">
-        <v>19</v>
+      <c r="P100" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q100" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C101" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D101" s="0" t="s">
-        <v>18</v>
+      <c r="C101" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E101" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F101" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G101" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H101" s="0" t="s">
-        <v>19</v>
+      <c r="F101" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G101" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H101" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I101" s="0" t="n">
         <v>60.23</v>
@@ -5892,8 +5883,8 @@
       <c r="L101" s="0" t="n">
         <v>4.76</v>
       </c>
-      <c r="M101" s="0" t="s">
-        <v>19</v>
+      <c r="M101" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="N101" s="0" t="n">
         <v>-16.31</v>
@@ -5901,25 +5892,25 @@
       <c r="O101" s="0" t="n">
         <v>-76.54</v>
       </c>
-      <c r="P101" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q101" s="0" t="s">
-        <v>19</v>
+      <c r="P101" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q101" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C102" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D102" s="0" t="s">
-        <v>18</v>
+      <c r="C102" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D102" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E102" s="0" t="n">
         <v>2</v>
@@ -5927,11 +5918,11 @@
       <c r="F102" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G102" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H102" s="0" t="s">
-        <v>19</v>
+      <c r="G102" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H102" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I102" s="0" t="n">
         <v>63.96</v>
@@ -5945,8 +5936,8 @@
       <c r="L102" s="0" t="n">
         <v>5.66</v>
       </c>
-      <c r="M102" s="0" t="s">
-        <v>19</v>
+      <c r="M102" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="N102" s="0" t="n">
         <v>28.15</v>
@@ -5954,16 +5945,16 @@
       <c r="O102" s="0" t="n">
         <v>-35.81</v>
       </c>
-      <c r="P102" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q102" s="0" t="s">
-        <v>19</v>
+      <c r="P102" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q102" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>4</v>
@@ -5977,8 +5968,8 @@
       <c r="E103" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F103" s="0" t="s">
-        <v>18</v>
+      <c r="F103" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G103" s="0" t="n">
         <v>-59.62</v>
@@ -6016,28 +6007,28 @@
     </row>
     <row r="104" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C104" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D104" s="0" t="s">
-        <v>18</v>
+      <c r="C104" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D104" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E104" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F104" s="0" t="s">
-        <v>18</v>
+      <c r="F104" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G104" s="0" t="n">
         <v>-52.78</v>
       </c>
-      <c r="H104" s="0" t="s">
-        <v>19</v>
+      <c r="H104" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I104" s="0" t="n">
         <v>41.78</v>
@@ -6060,25 +6051,25 @@
       <c r="O104" s="0" t="n">
         <v>-46.18</v>
       </c>
-      <c r="P104" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q104" s="0" t="s">
-        <v>19</v>
+      <c r="P104" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q104" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B105" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C105" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D105" s="0" t="s">
-        <v>18</v>
+      <c r="C105" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E105" s="0" t="n">
         <v>3</v>
@@ -6113,25 +6104,25 @@
       <c r="O105" s="0" t="n">
         <v>-50.4</v>
       </c>
-      <c r="P105" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q105" s="0" t="s">
-        <v>19</v>
+      <c r="P105" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q105" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C106" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D106" s="0" t="s">
-        <v>18</v>
+      <c r="C106" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D106" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E106" s="0" t="n">
         <v>1</v>
@@ -6175,7 +6166,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>4</v>
@@ -6228,19 +6219,19 @@
     </row>
     <row r="108" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B108" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C108" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D108" s="0" t="s">
-        <v>18</v>
+      <c r="C108" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D108" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E108" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F108" s="0" t="n">
         <v>3</v>
@@ -6263,8 +6254,8 @@
       <c r="L108" s="0" t="n">
         <v>2.92</v>
       </c>
-      <c r="M108" s="0" t="s">
-        <v>19</v>
+      <c r="M108" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="N108" s="0" t="n">
         <v>3.22</v>
@@ -6272,25 +6263,25 @@
       <c r="O108" s="0" t="n">
         <v>-45.12</v>
       </c>
-      <c r="P108" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q108" s="0" t="s">
-        <v>19</v>
+      <c r="P108" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q108" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C109" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D109" s="0" t="s">
-        <v>18</v>
+      <c r="C109" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D109" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E109" s="0" t="n">
         <v>1</v>
@@ -6298,11 +6289,11 @@
       <c r="F109" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G109" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H109" s="0" t="s">
-        <v>19</v>
+      <c r="G109" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H109" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I109" s="0" t="n">
         <v>49.72</v>
@@ -6325,25 +6316,25 @@
       <c r="O109" s="0" t="n">
         <v>-51.49</v>
       </c>
-      <c r="P109" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q109" s="0" t="s">
-        <v>19</v>
+      <c r="P109" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q109" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B110" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C110" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D110" s="0" t="s">
-        <v>18</v>
+      <c r="C110" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D110" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E110" s="0" t="n">
         <v>3</v>
@@ -6387,16 +6378,16 @@
     </row>
     <row r="111" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B111" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C111" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D111" s="0" t="s">
-        <v>18</v>
+      <c r="C111" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D111" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E111" s="0" t="n">
         <v>3</v>
@@ -6431,16 +6422,16 @@
       <c r="O111" s="0" t="n">
         <v>-47.29</v>
       </c>
-      <c r="P111" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q111" s="0" t="s">
-        <v>19</v>
+      <c r="P111" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q111" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B112" s="0" t="n">
         <v>4</v>
@@ -6493,7 +6484,7 @@
     </row>
     <row r="113" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>4</v>
@@ -6507,8 +6498,8 @@
       <c r="E113" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F113" s="0" t="s">
-        <v>18</v>
+      <c r="F113" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G113" s="0" t="n">
         <v>-40.72</v>
@@ -6546,22 +6537,22 @@
     </row>
     <row r="114" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C114" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D114" s="0" t="s">
-        <v>18</v>
+      <c r="C114" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D114" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E114" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F114" s="0" t="s">
-        <v>18</v>
+      <c r="F114" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G114" s="0" t="n">
         <v>-52.34</v>
@@ -6599,22 +6590,22 @@
     </row>
     <row r="115" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B115" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C115" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D115" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E115" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F115" s="0" t="s">
-        <v>18</v>
+      <c r="C115" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D115" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E115" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F115" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G115" s="0" t="n">
         <v>-54.2</v>
@@ -6652,28 +6643,28 @@
     </row>
     <row r="116" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B116" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C116" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D116" s="0" t="s">
-        <v>18</v>
+      <c r="C116" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D116" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E116" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F116" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G116" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H116" s="0" t="s">
-        <v>19</v>
+      <c r="F116" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G116" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H116" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I116" s="0" t="n">
         <v>51.47</v>
@@ -6696,31 +6687,31 @@
       <c r="O116" s="0" t="n">
         <v>-49.61</v>
       </c>
-      <c r="P116" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q116" s="0" t="s">
-        <v>19</v>
+      <c r="P116" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q116" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B117" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C117" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D117" s="0" t="s">
-        <v>18</v>
+      <c r="C117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D117" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E117" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F117" s="0" t="s">
-        <v>18</v>
+      <c r="F117" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G117" s="0" t="n">
         <v>-76.81</v>
@@ -6728,52 +6719,52 @@
       <c r="H117" s="0" t="n">
         <v>60.74</v>
       </c>
-      <c r="I117" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J117" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K117" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="L117" s="0" t="s">
-        <v>19</v>
+      <c r="I117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L117" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="M117" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N117" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="O117" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="P117" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q117" s="0" t="s">
-        <v>19</v>
+      <c r="N117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q117" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B118" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C118" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D118" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E118" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F118" s="0" t="s">
-        <v>18</v>
+      <c r="C118" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D118" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F118" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G118" s="0" t="n">
         <v>-42.24</v>
@@ -6811,22 +6802,22 @@
     </row>
     <row r="119" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C119" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D119" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E119" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F119" s="0" t="s">
-        <v>18</v>
+      <c r="C119" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D119" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E119" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F119" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G119" s="0" t="n">
         <v>-58.94</v>
@@ -6864,22 +6855,22 @@
     </row>
     <row r="120" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B120" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C120" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D120" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E120" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F120" s="0" t="s">
-        <v>18</v>
+      <c r="C120" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D120" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E120" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F120" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G120" s="0" t="n">
         <v>-54.63</v>
@@ -6896,8 +6887,8 @@
       <c r="K120" s="0" t="n">
         <v>9.42</v>
       </c>
-      <c r="L120" s="0" t="s">
-        <v>19</v>
+      <c r="L120" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="M120" s="0" t="n">
         <v>0</v>
@@ -6917,22 +6908,22 @@
     </row>
     <row r="121" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B121" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C121" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D121" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E121" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F121" s="0" t="s">
-        <v>18</v>
+      <c r="C121" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D121" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F121" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G121" s="0" t="n">
         <v>-57.34</v>
@@ -6970,7 +6961,7 @@
     </row>
     <row r="122" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B122" s="0" t="n">
         <v>4</v>
@@ -6978,14 +6969,14 @@
       <c r="C122" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D122" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E122" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F122" s="0" t="s">
-        <v>18</v>
+      <c r="D122" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F122" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G122" s="0" t="n">
         <v>-63.38</v>
@@ -6993,26 +6984,26 @@
       <c r="H122" s="0" t="n">
         <v>80.66</v>
       </c>
-      <c r="I122" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J122" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K122" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="L122" s="0" t="s">
-        <v>19</v>
+      <c r="I122" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J122" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K122" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L122" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="M122" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="N122" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="O122" s="0" t="s">
-        <v>19</v>
+      <c r="N122" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O122" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="P122" s="0" t="n">
         <v>28</v>
@@ -7023,22 +7014,22 @@
     </row>
     <row r="123" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B123" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C123" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D123" s="0" t="s">
-        <v>18</v>
+      <c r="C123" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D123" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E123" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F123" s="0" t="s">
-        <v>18</v>
+      <c r="F123" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="G123" s="0" t="n">
         <v>-58.89</v>
@@ -7076,16 +7067,16 @@
     </row>
     <row r="124" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B124" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C124" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D124" s="0" t="s">
-        <v>18</v>
+      <c r="C124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D124" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E124" s="0" t="n">
         <v>2</v>
@@ -7120,11 +7111,11 @@
       <c r="O124" s="0" t="n">
         <v>-56.28</v>
       </c>
-      <c r="P124" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q124" s="0" t="s">
-        <v>19</v>
+      <c r="P124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q124" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7150,9 +7141,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.54081632653061"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -7176,9 +7164,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.54081632653061"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>